<commit_message>
UI work is done
</commit_message>
<xml_diff>
--- a/Project Plan/UI Pages.xlsx
+++ b/Project Plan/UI Pages.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Sayfa 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sayfa 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>Tablo 1</t>
   </si>
@@ -155,11 +157,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -171,7 +170,7 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
@@ -312,61 +311,61 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -376,26 +375,82 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -521,7 +576,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -530,7 +585,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -539,7 +594,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -603,8 +658,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -612,7 +667,7 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
@@ -620,7 +675,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -639,7 +694,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -647,7 +702,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -675,7 +730,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -701,7 +756,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -727,7 +782,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -753,7 +808,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -779,7 +834,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -805,7 +860,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -831,7 +886,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -857,7 +912,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -883,7 +938,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -896,9 +951,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -915,7 +976,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -934,7 +995,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -960,7 +1021,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -986,7 +1047,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1012,7 +1073,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1038,7 +1099,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1064,7 +1125,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1090,7 +1151,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1116,7 +1177,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1142,7 +1203,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1168,7 +1229,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1181,9 +1242,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1197,7 +1264,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1216,7 +1283,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1246,7 +1313,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1272,7 +1339,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1298,7 +1365,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1324,7 +1391,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1350,7 +1417,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1376,7 +1443,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1402,7 +1469,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1428,7 +1495,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1454,7 +1521,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1467,447 +1534,459 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:G26"/>
+  <dimension ref="A1:IV26"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.41406" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.4297" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7812" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.3516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="1" customWidth="1"/>
+    <col min="4" max="256" width="16.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+    </row>
+    <row r="2" spans="1:7" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" ht="20.55" customHeight="1">
-      <c r="A3" s="5">
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="6">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="7">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s" s="7">
+      <c r="D3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>1</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" s="10">
+      <c r="F3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" t="s" s="11">
+      <c r="B4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s" s="12">
+      <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s" s="12">
+      <c r="D4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="12">
         <v>1</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" s="10">
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" t="s" s="11">
+      <c r="B5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s" s="12">
+      <c r="C5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s" s="12">
+      <c r="D5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <v>1</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" s="10">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" t="s" s="11">
+      <c r="B6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s" s="12">
+      <c r="C6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s" s="12">
+      <c r="D6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <v>1</v>
       </c>
-      <c r="F6" t="s" s="12">
+      <c r="F6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="14"/>
-    </row>
-    <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" s="10">
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
         <v>5</v>
       </c>
-      <c r="B7" t="s" s="11">
+      <c r="B7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s" s="12">
+      <c r="C7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s" s="12">
+      <c r="D7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>1</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" s="10">
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
         <v>6</v>
       </c>
-      <c r="B8" t="s" s="11">
+      <c r="B8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s" s="12">
+      <c r="C8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D8" t="s" s="12">
+      <c r="D8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>1</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-    </row>
-    <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" s="10">
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
         <v>7</v>
       </c>
-      <c r="B9" t="s" s="11">
+      <c r="B9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C9" t="s" s="12">
+      <c r="C9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s" s="12">
+      <c r="D9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <v>1</v>
       </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="10">
+      <c r="F9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
         <v>8</v>
       </c>
-      <c r="B10" t="s" s="11">
+      <c r="B10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s" s="12">
+      <c r="C10" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-    </row>
-    <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" s="10">
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
         <v>9</v>
       </c>
-      <c r="B11" t="s" s="11">
+      <c r="B11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s" s="12">
+      <c r="C11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" ht="20.35" customHeight="1">
-      <c r="A12" s="10">
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
         <v>10</v>
       </c>
-      <c r="B12" t="s" s="11">
+      <c r="B12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C12" t="s" s="12">
+      <c r="C12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-    </row>
-    <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" s="10">
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
         <v>11</v>
       </c>
-      <c r="B13" t="s" s="11">
+      <c r="B13" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C13" t="s" s="12">
+      <c r="C13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-    </row>
-    <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" s="10">
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="9">
         <v>12</v>
       </c>
-      <c r="B14" t="s" s="11">
+      <c r="B14" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C14" t="s" s="12">
+      <c r="C14" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-    </row>
-    <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="10">
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
         <v>13</v>
       </c>
-      <c r="B15" t="s" s="11">
+      <c r="B15" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C15" t="s" s="12">
+      <c r="C15" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-    </row>
-    <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" s="10">
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
         <v>14</v>
       </c>
-      <c r="B16" t="s" s="11">
+      <c r="B16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C16" t="s" s="12">
+      <c r="C16" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" s="10">
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
         <v>15</v>
       </c>
-      <c r="B17" t="s" s="11">
+      <c r="B17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C17" t="s" s="12">
+      <c r="C17" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" s="10">
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
         <v>16</v>
       </c>
-      <c r="B18" t="s" s="11">
+      <c r="B18" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C18" t="s" s="12">
+      <c r="C18" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-    </row>
-    <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" s="10">
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="9">
         <v>17</v>
       </c>
-      <c r="B19" t="s" s="11">
+      <c r="B19" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C19" t="s" s="12">
+      <c r="C19" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D19" t="s" s="12">
+      <c r="D19" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="12">
         <v>1</v>
       </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-    </row>
-    <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" s="10">
+      <c r="F19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s" s="11">
+      <c r="G19" s="13"/>
+    </row>
+    <row r="20" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="9">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C20" t="s" s="12">
+      <c r="C20" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-    </row>
-    <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" s="10">
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+    </row>
+    <row r="21" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="9">
         <v>19</v>
       </c>
-      <c r="B21" t="s" s="11">
+      <c r="B21" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C21" t="s" s="12">
+      <c r="C21" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D21" t="s" s="12">
+      <c r="D21" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="12">
         <v>1</v>
       </c>
-      <c r="F21" t="s" s="12">
+      <c r="F21" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="14"/>
-    </row>
-    <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" ht="20.35" customHeight="1">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-    </row>
-    <row r="24" ht="20.35" customHeight="1">
-      <c r="A24" s="15"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-    </row>
-    <row r="25" ht="20.35" customHeight="1">
-      <c r="A25" s="15"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-    </row>
-    <row r="26" ht="20.35" customHeight="1">
-      <c r="A26" s="15"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
+      <c r="G21" s="13"/>
+    </row>
+    <row r="22" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+    </row>
+    <row r="24" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="14"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+    </row>
+    <row r="25" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="14"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+    </row>
+    <row r="26" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="14"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
UI Pages priority updated.
</commit_message>
<xml_diff>
--- a/Project Plan/UI Pages.xlsx
+++ b/Project Plan/UI Pages.xlsx
@@ -1,20 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sayfa 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sayfa 1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
   <si>
     <t>Tablo 1</t>
   </si>
@@ -157,8 +155,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="0" formatCode="General"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -170,13 +171,18 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <b/>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,8 +201,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -208,6 +220,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -221,7 +255,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -230,7 +264,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -239,43 +273,43 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -284,88 +318,100 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -375,82 +421,28 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFBDC0BF"/>
-      <rgbColor rgb="FFA5A5A5"/>
-      <rgbColor rgb="FF3F3F3F"/>
-      <rgbColor rgb="FFDBDBDB"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -460,10 +452,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="404040"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="BFBFBF"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="499BC9"/>
@@ -576,7 +568,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -585,7 +577,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -594,7 +586,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -657,17 +649,18 @@
   <a:objectDefaults>
     <a:spDef>
       <a:spPr>
-        <a:blipFill rotWithShape="1">
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-          <a:srcRect/>
-          <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
-        </a:blipFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
@@ -675,39 +668,33 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst>
-              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="31034"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
             <a:uFillTx/>
             <a:latin typeface="+mn-lt"/>
             <a:ea typeface="+mn-ea"/>
@@ -730,7 +717,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -756,7 +743,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -782,7 +769,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -808,7 +795,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -834,7 +821,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -860,7 +847,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -886,7 +873,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -912,7 +899,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -938,7 +925,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -951,32 +938,32 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="6350" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="50000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -995,7 +982,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1021,7 +1008,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1047,7 +1034,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1073,7 +1060,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1099,7 +1086,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1125,7 +1112,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1151,7 +1138,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1177,7 +1164,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1203,7 +1190,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1229,7 +1216,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1242,15 +1229,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1264,26 +1245,26 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1313,7 +1294,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1339,7 +1320,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1365,7 +1346,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1391,7 +1372,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1417,7 +1398,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1443,7 +1424,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1469,7 +1450,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1495,7 +1476,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1521,7 +1502,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1534,459 +1515,465 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="1" customWidth="1"/>
-    <col min="4" max="256" width="16.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.35156" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.8516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.3516" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.3516" style="1" customWidth="1"/>
+    <col min="8" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+    <row r="1" ht="28" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-    </row>
-    <row r="2" spans="1:7" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" ht="20.55" customHeight="1">
+      <c r="A2" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s" s="5">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" ht="20.55" customHeight="1">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s" s="8">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" t="s" s="9">
         <v>8</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" t="s" s="9">
         <v>9</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="10">
         <v>1</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" ht="20.35" customHeight="1">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="E4" s="14">
+        <v>1</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+    </row>
+    <row r="5" ht="20.35" customHeight="1">
+      <c r="A5" s="11">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s" s="12">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s" s="13">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="E5" s="14">
+        <v>1</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" ht="20.35" customHeight="1">
+      <c r="A6" s="11">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s" s="13">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s" s="13">
+        <v>17</v>
+      </c>
+      <c r="E6" s="14">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s" s="13">
         <v>18</v>
       </c>
-      <c r="G3" s="8"/>
-    </row>
-    <row r="4" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" ht="20.35" customHeight="1">
+      <c r="A7" s="11">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s" s="12">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s" s="13">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s" s="13">
+        <v>21</v>
+      </c>
+      <c r="E7" s="14">
+        <v>1</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" ht="20.35" customHeight="1">
+      <c r="A8" s="11">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s" s="12">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s" s="13">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s" s="13">
+        <v>21</v>
+      </c>
+      <c r="E8" s="14">
+        <v>1</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" ht="20.35" customHeight="1">
+      <c r="A9" s="11">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s" s="12">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s" s="13">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="E9" s="14">
+        <v>1</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" ht="20.35" customHeight="1">
+      <c r="A10" s="11">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s" s="12">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s" s="13">
+        <v>26</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" ht="20.35" customHeight="1">
+      <c r="A11" s="11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s" s="12">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s" s="13">
+        <v>28</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14">
+        <v>2</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" ht="20.35" customHeight="1">
+      <c r="A12" s="11">
         <v>10</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="B12" t="s" s="12">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s" s="13">
+        <v>30</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14">
+        <v>2</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" ht="20.35" customHeight="1">
+      <c r="A13" s="11">
         <v>11</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="B13" t="s" s="12">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s" s="13">
+        <v>32</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14">
+        <v>2</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" ht="20.35" customHeight="1">
+      <c r="A14" s="11">
         <v>12</v>
       </c>
-      <c r="E4" s="12">
+      <c r="B14" t="s" s="12">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s" s="13">
+        <v>30</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14">
+        <v>2</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" ht="20.35" customHeight="1">
+      <c r="A15" s="11">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s" s="12">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s" s="13">
+        <v>23</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14">
         <v>1</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" ht="20.35" customHeight="1">
+      <c r="A16" s="11">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s" s="12">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s" s="13">
+        <v>36</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14">
+        <v>2</v>
+      </c>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" ht="20.35" customHeight="1">
+      <c r="A17" s="11">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s" s="12">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s" s="13">
+        <v>38</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="12">
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" ht="20.35" customHeight="1">
+      <c r="A18" s="11">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s" s="12">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s" s="13">
+        <v>36</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14">
+        <v>3</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" ht="20.35" customHeight="1">
+      <c r="A19" s="11">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s" s="12">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s" s="13">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="E19" s="14">
         <v>1</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-    </row>
-    <row r="6" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9">
-        <v>4</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="11" t="s">
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" ht="20.35" customHeight="1">
+      <c r="A20" s="11">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s" s="12">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s" s="13">
+        <v>43</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14">
+        <v>2</v>
+      </c>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" ht="20.35" customHeight="1">
+      <c r="A21" s="11">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s" s="12">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s" s="13">
+        <v>45</v>
+      </c>
+      <c r="D21" t="s" s="13">
         <v>17</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E21" s="14">
         <v>1</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F21" t="s" s="13">
         <v>18</v>
       </c>
-      <c r="G6" s="13"/>
-    </row>
-    <row r="7" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9">
-        <v>5</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="12">
-        <v>1</v>
-      </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-    </row>
-    <row r="8" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
-        <v>6</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="12">
-        <v>1</v>
-      </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="12">
-        <v>1</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
-        <v>8</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
-        <v>9</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
-        <v>10</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
-        <v>11</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9">
-        <v>12</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
-        <v>13</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
-        <v>14</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
-        <v>15</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
-        <v>16</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9">
-        <v>17</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="12">
-        <v>1</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9">
-        <v>18</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-    </row>
-    <row r="21" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9">
-        <v>19</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="12">
-        <v>1</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="13"/>
-    </row>
-    <row r="22" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" ht="20.35" customHeight="1">
+      <c r="A22" s="11"/>
       <c r="B22" s="15"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-    </row>
-    <row r="23" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" ht="20.35" customHeight="1">
+      <c r="A23" s="11"/>
       <c r="B23" s="15"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-    </row>
-    <row r="24" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+    </row>
+    <row r="24" ht="20.35" customHeight="1">
+      <c r="A24" s="11"/>
       <c r="B24" s="15"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-    </row>
-    <row r="25" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+    </row>
+    <row r="25" ht="20.35" customHeight="1">
+      <c r="A25" s="11"/>
       <c r="B25" s="15"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-    </row>
-    <row r="26" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+    </row>
+    <row r="26" ht="20.35" customHeight="1">
+      <c r="A26" s="11"/>
       <c r="B26" s="15"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>